<commit_message>
Update robustness + abstraction for Shein, Miravia, Tiktok marketplaces
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="1044">
   <si>
     <t>CÓDIGO</t>
   </si>
@@ -2213,6 +2213,9 @@
   </si>
   <si>
     <t>BY-BER05G</t>
+  </si>
+  <si>
+    <t>BY-BER90G</t>
   </si>
   <si>
     <t>BY-BHC007H</t>
@@ -3685,7 +3688,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E322" displayName="Tabla_1" name="Tabla_1" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E323" displayName="Tabla_1" name="Tabla_1" id="2">
   <tableColumns count="5">
     <tableColumn name="old_sku" id="1"/>
     <tableColumn name="new_sku" id="2"/>
@@ -10445,7 +10448,7 @@
         <v>733</v>
       </c>
       <c r="B77" s="28" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C77" s="29"/>
       <c r="D77" s="29"/>
@@ -10456,7 +10459,7 @@
         <v>734</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C78" s="29"/>
       <c r="D78" s="29"/>
@@ -10467,7 +10470,7 @@
         <v>735</v>
       </c>
       <c r="B79" s="28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C79" s="29"/>
       <c r="D79" s="29"/>
@@ -10478,28 +10481,26 @@
         <v>736</v>
       </c>
       <c r="B80" s="28" t="s">
-        <v>724</v>
+        <v>40</v>
       </c>
       <c r="C80" s="29"/>
       <c r="D80" s="29"/>
       <c r="E80" s="29"/>
     </row>
     <row r="81" ht="22.5" customHeight="1">
-      <c r="A81" s="31" t="s">
+      <c r="A81" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="B81" s="31" t="s">
-        <v>699</v>
-      </c>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="32" t="s">
-        <v>738</v>
-      </c>
+      <c r="B81" s="28" t="s">
+        <v>724</v>
+      </c>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
     </row>
     <row r="82" ht="22.5" customHeight="1">
       <c r="A82" s="31" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B82" s="31" t="s">
         <v>699</v>
@@ -10507,7 +10508,7 @@
       <c r="C82" s="32"/>
       <c r="D82" s="32"/>
       <c r="E82" s="32" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="83" ht="22.5" customHeight="1">
@@ -10515,31 +10516,33 @@
         <v>740</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="C83" s="32"/>
       <c r="D83" s="32"/>
       <c r="E83" s="32" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="84" ht="22.5" customHeight="1">
-      <c r="A84" s="28" t="s">
+      <c r="A84" s="31" t="s">
         <v>741</v>
       </c>
-      <c r="B84" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C84" s="29"/>
-      <c r="D84" s="29"/>
-      <c r="E84" s="29"/>
+      <c r="B84" s="31" t="s">
+        <v>704</v>
+      </c>
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
+      <c r="E84" s="32" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="85" ht="22.5" customHeight="1">
       <c r="A85" s="28" t="s">
         <v>742</v>
       </c>
       <c r="B85" s="28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C85" s="29"/>
       <c r="D85" s="29"/>
@@ -10550,7 +10553,7 @@
         <v>743</v>
       </c>
       <c r="B86" s="28" t="s">
-        <v>152</v>
+        <v>48</v>
       </c>
       <c r="C86" s="29"/>
       <c r="D86" s="29"/>
@@ -10561,7 +10564,7 @@
         <v>744</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="C87" s="29"/>
       <c r="D87" s="29"/>
@@ -10572,7 +10575,7 @@
         <v>745</v>
       </c>
       <c r="B88" s="28" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="29"/>
@@ -10583,7 +10586,7 @@
         <v>746</v>
       </c>
       <c r="B89" s="28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C89" s="29"/>
       <c r="D89" s="29"/>
@@ -10594,7 +10597,7 @@
         <v>747</v>
       </c>
       <c r="B90" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C90" s="29"/>
       <c r="D90" s="29"/>
@@ -10605,7 +10608,7 @@
         <v>748</v>
       </c>
       <c r="B91" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C91" s="29"/>
       <c r="D91" s="29"/>
@@ -10616,7 +10619,7 @@
         <v>749</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C92" s="29"/>
       <c r="D92" s="29"/>
@@ -10627,7 +10630,7 @@
         <v>750</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C93" s="29"/>
       <c r="D93" s="29"/>
@@ -10637,8 +10640,8 @@
       <c r="A94" s="28" t="s">
         <v>751</v>
       </c>
-      <c r="B94" s="33" t="s">
-        <v>66</v>
+      <c r="B94" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="C94" s="29"/>
       <c r="D94" s="29"/>
@@ -10648,8 +10651,8 @@
       <c r="A95" s="28" t="s">
         <v>752</v>
       </c>
-      <c r="B95" s="34" t="s">
-        <v>68</v>
+      <c r="B95" s="33" t="s">
+        <v>66</v>
       </c>
       <c r="C95" s="29"/>
       <c r="D95" s="29"/>
@@ -10660,7 +10663,7 @@
         <v>753</v>
       </c>
       <c r="B96" s="34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C96" s="29"/>
       <c r="D96" s="29"/>
@@ -10671,7 +10674,7 @@
         <v>754</v>
       </c>
       <c r="B97" s="34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C97" s="29"/>
       <c r="D97" s="29"/>
@@ -10682,7 +10685,7 @@
         <v>755</v>
       </c>
       <c r="B98" s="34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C98" s="29"/>
       <c r="D98" s="29"/>
@@ -10693,7 +10696,7 @@
         <v>756</v>
       </c>
       <c r="B99" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C99" s="29"/>
       <c r="D99" s="29"/>
@@ -10703,8 +10706,8 @@
       <c r="A100" s="28" t="s">
         <v>757</v>
       </c>
-      <c r="B100" s="28" t="s">
-        <v>78</v>
+      <c r="B100" s="34" t="s">
+        <v>76</v>
       </c>
       <c r="C100" s="29"/>
       <c r="D100" s="29"/>
@@ -10715,7 +10718,7 @@
         <v>758</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C101" s="29"/>
       <c r="D101" s="29"/>
@@ -10726,7 +10729,7 @@
         <v>759</v>
       </c>
       <c r="B102" s="28" t="s">
-        <v>760</v>
+        <v>86</v>
       </c>
       <c r="C102" s="29"/>
       <c r="D102" s="29"/>
@@ -10734,10 +10737,10 @@
     </row>
     <row r="103" ht="22.5" customHeight="1">
       <c r="A103" s="28" t="s">
+        <v>760</v>
+      </c>
+      <c r="B103" s="28" t="s">
         <v>761</v>
-      </c>
-      <c r="B103" s="28" t="s">
-        <v>98</v>
       </c>
       <c r="C103" s="29"/>
       <c r="D103" s="29"/>
@@ -10748,7 +10751,7 @@
         <v>762</v>
       </c>
       <c r="B104" s="28" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C104" s="29"/>
       <c r="D104" s="29"/>
@@ -10759,7 +10762,7 @@
         <v>763</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C105" s="29"/>
       <c r="D105" s="29"/>
@@ -10770,7 +10773,7 @@
         <v>764</v>
       </c>
       <c r="B106" s="28" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C106" s="29"/>
       <c r="D106" s="29"/>
@@ -10792,114 +10795,112 @@
         <v>766</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="C108" s="29"/>
       <c r="D108" s="29"/>
       <c r="E108" s="29"/>
     </row>
     <row r="109" ht="22.5" customHeight="1">
-      <c r="A109" s="31" t="s">
+      <c r="A109" s="28" t="s">
         <v>767</v>
       </c>
-      <c r="B109" s="35" t="s">
-        <v>768</v>
-      </c>
-      <c r="C109" s="36"/>
-      <c r="D109" s="36"/>
-      <c r="E109" s="32" t="s">
-        <v>769</v>
-      </c>
+      <c r="B109" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C109" s="29"/>
+      <c r="D109" s="29"/>
+      <c r="E109" s="29"/>
     </row>
     <row r="110" ht="22.5" customHeight="1">
       <c r="A110" s="31" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B110" s="35" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C110" s="36"/>
       <c r="D110" s="36"/>
       <c r="E110" s="32" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="111" ht="22.5" customHeight="1">
       <c r="A111" s="31" t="s">
+        <v>771</v>
+      </c>
+      <c r="B111" s="35" t="s">
         <v>772</v>
-      </c>
-      <c r="B111" s="35" t="s">
-        <v>773</v>
       </c>
       <c r="C111" s="36"/>
       <c r="D111" s="36"/>
       <c r="E111" s="32" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="112" ht="22.5" customHeight="1">
       <c r="A112" s="31" t="s">
+        <v>773</v>
+      </c>
+      <c r="B112" s="35" t="s">
         <v>774</v>
-      </c>
-      <c r="B112" s="35" t="s">
-        <v>775</v>
       </c>
       <c r="C112" s="36"/>
       <c r="D112" s="36"/>
       <c r="E112" s="32" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
     </row>
     <row r="113" ht="22.5" customHeight="1">
       <c r="A113" s="31" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B113" s="35" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C113" s="36"/>
       <c r="D113" s="36"/>
       <c r="E113" s="32" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="114" ht="22.5" customHeight="1">
       <c r="A114" s="31" t="s">
+        <v>778</v>
+      </c>
+      <c r="B114" s="35" t="s">
         <v>779</v>
-      </c>
-      <c r="B114" s="35" t="s">
-        <v>780</v>
       </c>
       <c r="C114" s="36"/>
       <c r="D114" s="36"/>
       <c r="E114" s="32" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="115" ht="22.5" customHeight="1">
       <c r="A115" s="31" t="s">
+        <v>780</v>
+      </c>
+      <c r="B115" s="35" t="s">
         <v>781</v>
-      </c>
-      <c r="B115" s="35" t="s">
-        <v>782</v>
       </c>
       <c r="C115" s="36"/>
       <c r="D115" s="36"/>
       <c r="E115" s="32" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="116" ht="22.5" customHeight="1">
       <c r="A116" s="31" t="s">
+        <v>782</v>
+      </c>
+      <c r="B116" s="35" t="s">
         <v>783</v>
-      </c>
-      <c r="B116" s="35" t="s">
-        <v>782</v>
       </c>
       <c r="C116" s="36"/>
       <c r="D116" s="36"/>
       <c r="E116" s="32" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="117" ht="22.5" customHeight="1">
@@ -10907,31 +10908,33 @@
         <v>784</v>
       </c>
       <c r="B117" s="35" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="C117" s="36"/>
       <c r="D117" s="36"/>
       <c r="E117" s="32" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="118" ht="22.5" customHeight="1">
-      <c r="A118" s="28" t="s">
+      <c r="A118" s="31" t="s">
         <v>785</v>
       </c>
-      <c r="B118" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="C118" s="29"/>
-      <c r="D118" s="29"/>
-      <c r="E118" s="29"/>
+      <c r="B118" s="35" t="s">
+        <v>781</v>
+      </c>
+      <c r="C118" s="36"/>
+      <c r="D118" s="36"/>
+      <c r="E118" s="32" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="119" ht="22.5" customHeight="1">
       <c r="A119" s="28" t="s">
         <v>786</v>
       </c>
       <c r="B119" s="28" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C119" s="29"/>
       <c r="D119" s="29"/>
@@ -10941,8 +10944,8 @@
       <c r="A120" s="28" t="s">
         <v>787</v>
       </c>
-      <c r="B120" s="33" t="s">
-        <v>78</v>
+      <c r="B120" s="28" t="s">
+        <v>152</v>
       </c>
       <c r="C120" s="29"/>
       <c r="D120" s="29"/>
@@ -10952,8 +10955,8 @@
       <c r="A121" s="28" t="s">
         <v>788</v>
       </c>
-      <c r="B121" s="28" t="s">
-        <v>60</v>
+      <c r="B121" s="33" t="s">
+        <v>78</v>
       </c>
       <c r="C121" s="29"/>
       <c r="D121" s="29"/>
@@ -10964,7 +10967,7 @@
         <v>789</v>
       </c>
       <c r="B122" s="28" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C122" s="29"/>
       <c r="D122" s="29"/>
@@ -10975,7 +10978,7 @@
         <v>790</v>
       </c>
       <c r="B123" s="28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C123" s="29"/>
       <c r="D123" s="29"/>
@@ -10986,7 +10989,7 @@
         <v>791</v>
       </c>
       <c r="B124" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C124" s="29"/>
       <c r="D124" s="29"/>
@@ -10997,7 +11000,7 @@
         <v>792</v>
       </c>
       <c r="B125" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C125" s="29"/>
       <c r="D125" s="29"/>
@@ -11008,7 +11011,7 @@
         <v>793</v>
       </c>
       <c r="B126" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C126" s="29"/>
       <c r="D126" s="29"/>
@@ -11019,7 +11022,7 @@
         <v>794</v>
       </c>
       <c r="B127" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C127" s="29"/>
       <c r="D127" s="29"/>
@@ -11029,8 +11032,8 @@
       <c r="A128" s="28" t="s">
         <v>795</v>
       </c>
-      <c r="B128" s="33" t="s">
-        <v>78</v>
+      <c r="B128" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="C128" s="29"/>
       <c r="D128" s="29"/>
@@ -11040,8 +11043,8 @@
       <c r="A129" s="28" t="s">
         <v>796</v>
       </c>
-      <c r="B129" s="28" t="s">
-        <v>110</v>
+      <c r="B129" s="33" t="s">
+        <v>78</v>
       </c>
       <c r="C129" s="29"/>
       <c r="D129" s="29"/>
@@ -11052,7 +11055,7 @@
         <v>797</v>
       </c>
       <c r="B130" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C130" s="29"/>
       <c r="D130" s="29"/>
@@ -11063,31 +11066,29 @@
         <v>798</v>
       </c>
       <c r="B131" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C131" s="29"/>
       <c r="D131" s="29"/>
       <c r="E131" s="29"/>
     </row>
     <row r="132" ht="22.5" customHeight="1">
-      <c r="A132" s="37" t="s">
+      <c r="A132" s="28" t="s">
         <v>799</v>
       </c>
-      <c r="B132" s="37" t="s">
-        <v>268</v>
-      </c>
-      <c r="C132" s="38"/>
-      <c r="D132" s="38">
-        <v>2.0</v>
-      </c>
-      <c r="E132" s="38"/>
+      <c r="B132" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C132" s="29"/>
+      <c r="D132" s="29"/>
+      <c r="E132" s="29"/>
     </row>
     <row r="133" ht="22.5" customHeight="1">
       <c r="A133" s="37" t="s">
         <v>800</v>
       </c>
       <c r="B133" s="37" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C133" s="38"/>
       <c r="D133" s="38">
@@ -11096,22 +11097,24 @@
       <c r="E133" s="38"/>
     </row>
     <row r="134" ht="22.5" customHeight="1">
-      <c r="A134" s="28" t="s">
+      <c r="A134" s="37" t="s">
         <v>801</v>
       </c>
-      <c r="B134" s="28" t="s">
-        <v>396</v>
-      </c>
-      <c r="C134" s="29"/>
-      <c r="D134" s="29"/>
-      <c r="E134" s="29"/>
+      <c r="B134" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="C134" s="38"/>
+      <c r="D134" s="38">
+        <v>2.0</v>
+      </c>
+      <c r="E134" s="38"/>
     </row>
     <row r="135" ht="22.5" customHeight="1">
       <c r="A135" s="28" t="s">
         <v>802</v>
       </c>
       <c r="B135" s="28" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C135" s="29"/>
       <c r="D135" s="29"/>
@@ -11122,7 +11125,7 @@
         <v>803</v>
       </c>
       <c r="B136" s="28" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C136" s="29"/>
       <c r="D136" s="29"/>
@@ -11133,7 +11136,7 @@
         <v>804</v>
       </c>
       <c r="B137" s="28" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C137" s="29"/>
       <c r="D137" s="29"/>
@@ -11144,7 +11147,7 @@
         <v>805</v>
       </c>
       <c r="B138" s="28" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C138" s="29"/>
       <c r="D138" s="29"/>
@@ -11155,26 +11158,26 @@
         <v>806</v>
       </c>
       <c r="B139" s="28" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C139" s="29"/>
       <c r="D139" s="29"/>
       <c r="E139" s="29"/>
     </row>
     <row r="140" ht="22.5" customHeight="1">
-      <c r="A140" s="39" t="s">
-        <v>286</v>
-      </c>
-      <c r="B140" s="40"/>
-      <c r="C140" s="41"/>
-      <c r="D140" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="E140" s="41"/>
+      <c r="A140" s="28" t="s">
+        <v>807</v>
+      </c>
+      <c r="B140" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="C140" s="29"/>
+      <c r="D140" s="29"/>
+      <c r="E140" s="29"/>
     </row>
     <row r="141" ht="22.5" customHeight="1">
       <c r="A141" s="39" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B141" s="40"/>
       <c r="C141" s="41"/>
@@ -11185,7 +11188,7 @@
     </row>
     <row r="142" ht="22.5" customHeight="1">
       <c r="A142" s="39" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B142" s="40"/>
       <c r="C142" s="41"/>
@@ -11196,7 +11199,7 @@
     </row>
     <row r="143" ht="22.5" customHeight="1">
       <c r="A143" s="39" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B143" s="40"/>
       <c r="C143" s="41"/>
@@ -11207,7 +11210,7 @@
     </row>
     <row r="144" ht="22.5" customHeight="1">
       <c r="A144" s="39" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B144" s="40"/>
       <c r="C144" s="41"/>
@@ -11218,7 +11221,7 @@
     </row>
     <row r="145" ht="22.5" customHeight="1">
       <c r="A145" s="39" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B145" s="40"/>
       <c r="C145" s="41"/>
@@ -11228,15 +11231,15 @@
       <c r="E145" s="41"/>
     </row>
     <row r="146" ht="22.5" customHeight="1">
-      <c r="A146" s="42" t="s">
-        <v>807</v>
-      </c>
-      <c r="B146" s="43"/>
-      <c r="C146" s="44" t="s">
-        <v>328</v>
-      </c>
-      <c r="D146" s="43"/>
-      <c r="E146" s="43"/>
+      <c r="A146" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="B146" s="40"/>
+      <c r="C146" s="41"/>
+      <c r="D146" s="41">
+        <v>2.0</v>
+      </c>
+      <c r="E146" s="41"/>
     </row>
     <row r="147" ht="22.5" customHeight="1">
       <c r="A147" s="42" t="s">
@@ -11277,7 +11280,7 @@
       </c>
       <c r="B150" s="43"/>
       <c r="C150" s="44" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D150" s="43"/>
       <c r="E150" s="43"/>
@@ -11327,35 +11330,33 @@
       <c r="E154" s="43"/>
     </row>
     <row r="155" ht="22.5" customHeight="1">
-      <c r="A155" s="28" t="s">
+      <c r="A155" s="42" t="s">
         <v>816</v>
       </c>
-      <c r="B155" s="28" t="s">
+      <c r="B155" s="43"/>
+      <c r="C155" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="D155" s="43"/>
+      <c r="E155" s="43"/>
+    </row>
+    <row r="156" ht="22.5" customHeight="1">
+      <c r="A156" s="28" t="s">
+        <v>817</v>
+      </c>
+      <c r="B156" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="C155" s="29"/>
-      <c r="D155" s="29"/>
-      <c r="E155" s="29"/>
-    </row>
-    <row r="156" ht="22.5" customHeight="1">
-      <c r="A156" s="37" t="s">
-        <v>817</v>
-      </c>
-      <c r="B156" s="45" t="s">
-        <v>416</v>
-      </c>
-      <c r="C156" s="38"/>
-      <c r="D156" s="38">
-        <v>10.0</v>
-      </c>
-      <c r="E156" s="38"/>
+      <c r="C156" s="29"/>
+      <c r="D156" s="29"/>
+      <c r="E156" s="29"/>
     </row>
     <row r="157" ht="22.5" customHeight="1">
       <c r="A157" s="37" t="s">
         <v>818</v>
       </c>
       <c r="B157" s="45" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C157" s="38"/>
       <c r="D157" s="38">
@@ -11368,7 +11369,7 @@
         <v>819</v>
       </c>
       <c r="B158" s="45" t="s">
-        <v>476</v>
+        <v>424</v>
       </c>
       <c r="C158" s="38"/>
       <c r="D158" s="38">
@@ -11381,7 +11382,7 @@
         <v>820</v>
       </c>
       <c r="B159" s="45" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C159" s="38"/>
       <c r="D159" s="38">
@@ -11394,11 +11395,11 @@
         <v>821</v>
       </c>
       <c r="B160" s="45" t="s">
-        <v>416</v>
+        <v>478</v>
       </c>
       <c r="C160" s="38"/>
       <c r="D160" s="38">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="E160" s="38"/>
     </row>
@@ -11407,7 +11408,7 @@
         <v>822</v>
       </c>
       <c r="B161" s="45" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C161" s="38"/>
       <c r="D161" s="38">
@@ -11420,7 +11421,7 @@
         <v>823</v>
       </c>
       <c r="B162" s="45" t="s">
-        <v>476</v>
+        <v>424</v>
       </c>
       <c r="C162" s="38"/>
       <c r="D162" s="38">
@@ -11433,7 +11434,7 @@
         <v>824</v>
       </c>
       <c r="B163" s="45" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C163" s="38"/>
       <c r="D163" s="38">
@@ -11446,11 +11447,11 @@
         <v>825</v>
       </c>
       <c r="B164" s="45" t="s">
-        <v>436</v>
+        <v>478</v>
       </c>
       <c r="C164" s="38"/>
       <c r="D164" s="38">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="E164" s="38"/>
     </row>
@@ -11459,7 +11460,7 @@
         <v>826</v>
       </c>
       <c r="B165" s="45" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C165" s="38"/>
       <c r="D165" s="38">
@@ -11472,7 +11473,7 @@
         <v>827</v>
       </c>
       <c r="B166" s="45" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C166" s="38"/>
       <c r="D166" s="38">
@@ -11485,7 +11486,7 @@
         <v>828</v>
       </c>
       <c r="B167" s="45" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C167" s="38"/>
       <c r="D167" s="38">
@@ -11498,7 +11499,7 @@
         <v>829</v>
       </c>
       <c r="B168" s="45" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C168" s="38"/>
       <c r="D168" s="38">
@@ -11511,7 +11512,7 @@
         <v>830</v>
       </c>
       <c r="B169" s="45" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="C169" s="38"/>
       <c r="D169" s="38">
@@ -11524,7 +11525,7 @@
         <v>831</v>
       </c>
       <c r="B170" s="45" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C170" s="38"/>
       <c r="D170" s="38">
@@ -11537,7 +11538,7 @@
         <v>832</v>
       </c>
       <c r="B171" s="45" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C171" s="38"/>
       <c r="D171" s="38">
@@ -11550,11 +11551,11 @@
         <v>833</v>
       </c>
       <c r="B172" s="45" t="s">
-        <v>416</v>
+        <v>462</v>
       </c>
       <c r="C172" s="38"/>
       <c r="D172" s="38">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E172" s="38"/>
     </row>
@@ -11563,7 +11564,7 @@
         <v>834</v>
       </c>
       <c r="B173" s="45" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C173" s="38"/>
       <c r="D173" s="38">
@@ -11576,7 +11577,7 @@
         <v>835</v>
       </c>
       <c r="B174" s="45" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="C174" s="38"/>
       <c r="D174" s="38">
@@ -11589,7 +11590,7 @@
         <v>836</v>
       </c>
       <c r="B175" s="45" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C175" s="38"/>
       <c r="D175" s="38">
@@ -11602,7 +11603,7 @@
         <v>837</v>
       </c>
       <c r="B176" s="45" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C176" s="38"/>
       <c r="D176" s="38">
@@ -11615,7 +11616,7 @@
         <v>838</v>
       </c>
       <c r="B177" s="45" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C177" s="38"/>
       <c r="D177" s="38">
@@ -11628,7 +11629,7 @@
         <v>839</v>
       </c>
       <c r="B178" s="45" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C178" s="38"/>
       <c r="D178" s="38">
@@ -11641,7 +11642,7 @@
         <v>840</v>
       </c>
       <c r="B179" s="45" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="C179" s="38"/>
       <c r="D179" s="38">
@@ -11654,7 +11655,7 @@
         <v>841</v>
       </c>
       <c r="B180" s="45" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C180" s="38"/>
       <c r="D180" s="38">
@@ -11667,7 +11668,7 @@
         <v>842</v>
       </c>
       <c r="B181" s="45" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C181" s="38"/>
       <c r="D181" s="38">
@@ -11680,7 +11681,7 @@
         <v>843</v>
       </c>
       <c r="B182" s="45" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="C182" s="38"/>
       <c r="D182" s="38">
@@ -11693,7 +11694,7 @@
         <v>844</v>
       </c>
       <c r="B183" s="45" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C183" s="38"/>
       <c r="D183" s="38">
@@ -11706,11 +11707,11 @@
         <v>845</v>
       </c>
       <c r="B184" s="45" t="s">
-        <v>416</v>
+        <v>478</v>
       </c>
       <c r="C184" s="38"/>
       <c r="D184" s="38">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="E184" s="38"/>
     </row>
@@ -11719,7 +11720,7 @@
         <v>846</v>
       </c>
       <c r="B185" s="45" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C185" s="38"/>
       <c r="D185" s="38">
@@ -11732,7 +11733,7 @@
         <v>847</v>
       </c>
       <c r="B186" s="45" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="C186" s="38"/>
       <c r="D186" s="38">
@@ -11758,7 +11759,7 @@
         <v>849</v>
       </c>
       <c r="B188" s="45" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C188" s="38"/>
       <c r="D188" s="38">
@@ -11771,7 +11772,7 @@
         <v>850</v>
       </c>
       <c r="B189" s="45" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C189" s="38"/>
       <c r="D189" s="38">
@@ -11784,7 +11785,7 @@
         <v>851</v>
       </c>
       <c r="B190" s="45" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C190" s="38"/>
       <c r="D190" s="38">
@@ -11797,7 +11798,7 @@
         <v>852</v>
       </c>
       <c r="B191" s="45" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="C191" s="38"/>
       <c r="D191" s="38">
@@ -11810,7 +11811,7 @@
         <v>853</v>
       </c>
       <c r="B192" s="45" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C192" s="38"/>
       <c r="D192" s="38">
@@ -11823,7 +11824,7 @@
         <v>854</v>
       </c>
       <c r="B193" s="45" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C193" s="38"/>
       <c r="D193" s="38">
@@ -11836,7 +11837,7 @@
         <v>855</v>
       </c>
       <c r="B194" s="45" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="C194" s="38"/>
       <c r="D194" s="38">
@@ -11849,7 +11850,7 @@
         <v>856</v>
       </c>
       <c r="B195" s="45" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C195" s="38"/>
       <c r="D195" s="38">
@@ -11862,11 +11863,11 @@
         <v>857</v>
       </c>
       <c r="B196" s="45" t="s">
-        <v>436</v>
+        <v>478</v>
       </c>
       <c r="C196" s="38"/>
       <c r="D196" s="38">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="E196" s="38"/>
     </row>
@@ -11875,7 +11876,7 @@
         <v>858</v>
       </c>
       <c r="B197" s="45" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C197" s="38"/>
       <c r="D197" s="38">
@@ -11888,7 +11889,7 @@
         <v>859</v>
       </c>
       <c r="B198" s="45" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C198" s="38"/>
       <c r="D198" s="38">
@@ -11901,7 +11902,7 @@
         <v>860</v>
       </c>
       <c r="B199" s="45" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C199" s="38"/>
       <c r="D199" s="38">
@@ -11914,7 +11915,7 @@
         <v>861</v>
       </c>
       <c r="B200" s="45" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C200" s="38"/>
       <c r="D200" s="38">
@@ -11927,7 +11928,7 @@
         <v>862</v>
       </c>
       <c r="B201" s="45" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="C201" s="38"/>
       <c r="D201" s="38">
@@ -11940,7 +11941,7 @@
         <v>863</v>
       </c>
       <c r="B202" s="45" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C202" s="38"/>
       <c r="D202" s="38">
@@ -11953,7 +11954,7 @@
         <v>864</v>
       </c>
       <c r="B203" s="45" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C203" s="38"/>
       <c r="D203" s="38">
@@ -11966,11 +11967,11 @@
         <v>865</v>
       </c>
       <c r="B204" s="45" t="s">
-        <v>416</v>
+        <v>462</v>
       </c>
       <c r="C204" s="38"/>
       <c r="D204" s="38">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="E204" s="38"/>
     </row>
@@ -11979,7 +11980,7 @@
         <v>866</v>
       </c>
       <c r="B205" s="45" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C205" s="38"/>
       <c r="D205" s="38">
@@ -11992,7 +11993,7 @@
         <v>867</v>
       </c>
       <c r="B206" s="45" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="C206" s="38"/>
       <c r="D206" s="38">
@@ -12005,7 +12006,7 @@
         <v>868</v>
       </c>
       <c r="B207" s="45" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C207" s="38"/>
       <c r="D207" s="38">
@@ -12018,7 +12019,7 @@
         <v>869</v>
       </c>
       <c r="B208" s="45" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C208" s="38"/>
       <c r="D208" s="38">
@@ -12031,7 +12032,7 @@
         <v>870</v>
       </c>
       <c r="B209" s="45" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C209" s="38"/>
       <c r="D209" s="38">
@@ -12044,7 +12045,7 @@
         <v>871</v>
       </c>
       <c r="B210" s="45" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C210" s="38"/>
       <c r="D210" s="38">
@@ -12057,7 +12058,7 @@
         <v>872</v>
       </c>
       <c r="B211" s="45" t="s">
-        <v>476</v>
+        <v>448</v>
       </c>
       <c r="C211" s="38"/>
       <c r="D211" s="38">
@@ -12070,7 +12071,7 @@
         <v>873</v>
       </c>
       <c r="B212" s="45" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C212" s="38"/>
       <c r="D212" s="38">
@@ -12083,11 +12084,11 @@
         <v>874</v>
       </c>
       <c r="B213" s="45" t="s">
-        <v>416</v>
+        <v>478</v>
       </c>
       <c r="C213" s="38"/>
       <c r="D213" s="38">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="E213" s="38"/>
     </row>
@@ -12096,7 +12097,7 @@
         <v>875</v>
       </c>
       <c r="B214" s="45" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C214" s="38"/>
       <c r="D214" s="38">
@@ -12109,7 +12110,7 @@
         <v>876</v>
       </c>
       <c r="B215" s="45" t="s">
-        <v>476</v>
+        <v>424</v>
       </c>
       <c r="C215" s="38"/>
       <c r="D215" s="38">
@@ -12122,7 +12123,7 @@
         <v>877</v>
       </c>
       <c r="B216" s="45" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C216" s="38"/>
       <c r="D216" s="38">
@@ -12131,22 +12132,24 @@
       <c r="E216" s="38"/>
     </row>
     <row r="217" ht="22.5" customHeight="1">
-      <c r="A217" s="28" t="s">
+      <c r="A217" s="37" t="s">
         <v>878</v>
       </c>
-      <c r="B217" s="33" t="s">
+      <c r="B217" s="45" t="s">
+        <v>478</v>
+      </c>
+      <c r="C217" s="38"/>
+      <c r="D217" s="38">
+        <v>8.0</v>
+      </c>
+      <c r="E217" s="38"/>
+    </row>
+    <row r="218" ht="22.5" customHeight="1">
+      <c r="A218" s="28" t="s">
+        <v>879</v>
+      </c>
+      <c r="B218" s="33" t="s">
         <v>416</v>
-      </c>
-      <c r="C217" s="30"/>
-      <c r="D217" s="30"/>
-      <c r="E217" s="30"/>
-    </row>
-    <row r="218" ht="22.5" customHeight="1">
-      <c r="A218" s="46" t="s">
-        <v>879</v>
-      </c>
-      <c r="B218" s="33" t="s">
-        <v>418</v>
       </c>
       <c r="C218" s="30"/>
       <c r="D218" s="30"/>
@@ -12157,7 +12160,7 @@
         <v>880</v>
       </c>
       <c r="B219" s="33" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C219" s="30"/>
       <c r="D219" s="30"/>
@@ -12168,7 +12171,7 @@
         <v>881</v>
       </c>
       <c r="B220" s="33" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C220" s="30"/>
       <c r="D220" s="30"/>
@@ -12179,7 +12182,7 @@
         <v>882</v>
       </c>
       <c r="B221" s="33" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C221" s="30"/>
       <c r="D221" s="30"/>
@@ -12190,7 +12193,7 @@
         <v>883</v>
       </c>
       <c r="B222" s="33" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C222" s="30"/>
       <c r="D222" s="30"/>
@@ -12201,7 +12204,7 @@
         <v>884</v>
       </c>
       <c r="B223" s="33" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="C223" s="30"/>
       <c r="D223" s="30"/>
@@ -12212,7 +12215,7 @@
         <v>885</v>
       </c>
       <c r="B224" s="33" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C224" s="30"/>
       <c r="D224" s="30"/>
@@ -12223,7 +12226,7 @@
         <v>886</v>
       </c>
       <c r="B225" s="33" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C225" s="30"/>
       <c r="D225" s="30"/>
@@ -12234,7 +12237,7 @@
         <v>887</v>
       </c>
       <c r="B226" s="33" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C226" s="30"/>
       <c r="D226" s="30"/>
@@ -12245,7 +12248,7 @@
         <v>888</v>
       </c>
       <c r="B227" s="33" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C227" s="30"/>
       <c r="D227" s="30"/>
@@ -12256,7 +12259,7 @@
         <v>889</v>
       </c>
       <c r="B228" s="33" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C228" s="30"/>
       <c r="D228" s="30"/>
@@ -12267,7 +12270,7 @@
         <v>890</v>
       </c>
       <c r="B229" s="33" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C229" s="30"/>
       <c r="D229" s="30"/>
@@ -12278,7 +12281,7 @@
         <v>891</v>
       </c>
       <c r="B230" s="33" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C230" s="30"/>
       <c r="D230" s="30"/>
@@ -12289,7 +12292,7 @@
         <v>892</v>
       </c>
       <c r="B231" s="33" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C231" s="30"/>
       <c r="D231" s="30"/>
@@ -12300,29 +12303,29 @@
         <v>893</v>
       </c>
       <c r="B232" s="33" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C232" s="30"/>
       <c r="D232" s="30"/>
       <c r="E232" s="30"/>
     </row>
     <row r="233" ht="22.5" customHeight="1">
-      <c r="A233" s="28" t="s">
+      <c r="A233" s="46" t="s">
         <v>894</v>
       </c>
       <c r="B233" s="33" t="s">
-        <v>604</v>
+        <v>462</v>
       </c>
       <c r="C233" s="30"/>
       <c r="D233" s="30"/>
       <c r="E233" s="30"/>
     </row>
     <row r="234" ht="22.5" customHeight="1">
-      <c r="A234" s="46" t="s">
+      <c r="A234" s="28" t="s">
         <v>895</v>
       </c>
       <c r="B234" s="33" t="s">
-        <v>468</v>
+        <v>604</v>
       </c>
       <c r="C234" s="30"/>
       <c r="D234" s="30"/>
@@ -12333,7 +12336,7 @@
         <v>896</v>
       </c>
       <c r="B235" s="33" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C235" s="30"/>
       <c r="D235" s="30"/>
@@ -12344,7 +12347,7 @@
         <v>897</v>
       </c>
       <c r="B236" s="33" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C236" s="30"/>
       <c r="D236" s="30"/>
@@ -12355,7 +12358,7 @@
         <v>898</v>
       </c>
       <c r="B237" s="33" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C237" s="30"/>
       <c r="D237" s="30"/>
@@ -12366,7 +12369,7 @@
         <v>899</v>
       </c>
       <c r="B238" s="33" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C238" s="30"/>
       <c r="D238" s="30"/>
@@ -12377,7 +12380,7 @@
         <v>900</v>
       </c>
       <c r="B239" s="33" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C239" s="30"/>
       <c r="D239" s="30"/>
@@ -12388,7 +12391,7 @@
         <v>901</v>
       </c>
       <c r="B240" s="33" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C240" s="30"/>
       <c r="D240" s="30"/>
@@ -12399,35 +12402,33 @@
         <v>902</v>
       </c>
       <c r="B241" s="33" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C241" s="30"/>
       <c r="D241" s="30"/>
       <c r="E241" s="30"/>
     </row>
     <row r="242" ht="22.5" customHeight="1">
-      <c r="A242" s="39" t="s">
+      <c r="A242" s="46" t="s">
+        <v>903</v>
+      </c>
+      <c r="B242" s="33" t="s">
+        <v>488</v>
+      </c>
+      <c r="C242" s="30"/>
+      <c r="D242" s="30"/>
+      <c r="E242" s="30"/>
+    </row>
+    <row r="243" ht="22.5" customHeight="1">
+      <c r="A243" s="39" t="s">
         <v>534</v>
       </c>
-      <c r="B242" s="40"/>
-      <c r="C242" s="41"/>
-      <c r="D242" s="41">
+      <c r="B243" s="40"/>
+      <c r="C243" s="41"/>
+      <c r="D243" s="41">
         <v>4.0</v>
       </c>
-      <c r="E242" s="41"/>
-    </row>
-    <row r="243" ht="22.5" customHeight="1">
-      <c r="A243" s="37" t="s">
-        <v>903</v>
-      </c>
-      <c r="B243" s="45" t="s">
-        <v>534</v>
-      </c>
-      <c r="C243" s="38"/>
-      <c r="D243" s="38">
-        <v>12.0</v>
-      </c>
-      <c r="E243" s="38"/>
+      <c r="E243" s="41"/>
     </row>
     <row r="244" ht="22.5" customHeight="1">
       <c r="A244" s="37" t="s">
@@ -12438,7 +12439,7 @@
       </c>
       <c r="C244" s="38"/>
       <c r="D244" s="38">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="E244" s="38"/>
     </row>
@@ -12451,7 +12452,7 @@
       </c>
       <c r="C245" s="38"/>
       <c r="D245" s="38">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="E245" s="38"/>
     </row>
@@ -12464,7 +12465,7 @@
       </c>
       <c r="C246" s="38"/>
       <c r="D246" s="38">
-        <v>24.0</v>
+        <v>20.0</v>
       </c>
       <c r="E246" s="38"/>
     </row>
@@ -12477,7 +12478,7 @@
       </c>
       <c r="C247" s="38"/>
       <c r="D247" s="38">
-        <v>28.0</v>
+        <v>24.0</v>
       </c>
       <c r="E247" s="38"/>
     </row>
@@ -12490,7 +12491,7 @@
       </c>
       <c r="C248" s="38"/>
       <c r="D248" s="38">
-        <v>32.0</v>
+        <v>28.0</v>
       </c>
       <c r="E248" s="38"/>
     </row>
@@ -12503,7 +12504,7 @@
       </c>
       <c r="C249" s="38"/>
       <c r="D249" s="38">
-        <v>36.0</v>
+        <v>32.0</v>
       </c>
       <c r="E249" s="38"/>
     </row>
@@ -12516,7 +12517,7 @@
       </c>
       <c r="C250" s="38"/>
       <c r="D250" s="38">
-        <v>4.0</v>
+        <v>36.0</v>
       </c>
       <c r="E250" s="38"/>
     </row>
@@ -12529,7 +12530,7 @@
       </c>
       <c r="C251" s="38"/>
       <c r="D251" s="38">
-        <v>40.0</v>
+        <v>4.0</v>
       </c>
       <c r="E251" s="38"/>
     </row>
@@ -12542,7 +12543,7 @@
       </c>
       <c r="C252" s="38"/>
       <c r="D252" s="38">
-        <v>44.0</v>
+        <v>40.0</v>
       </c>
       <c r="E252" s="38"/>
     </row>
@@ -12555,7 +12556,7 @@
       </c>
       <c r="C253" s="38"/>
       <c r="D253" s="38">
-        <v>48.0</v>
+        <v>44.0</v>
       </c>
       <c r="E253" s="38"/>
     </row>
@@ -12568,33 +12569,33 @@
       </c>
       <c r="C254" s="38"/>
       <c r="D254" s="38">
+        <v>48.0</v>
+      </c>
+      <c r="E254" s="38"/>
+    </row>
+    <row r="255" ht="22.5" customHeight="1">
+      <c r="A255" s="37" t="s">
+        <v>915</v>
+      </c>
+      <c r="B255" s="45" t="s">
+        <v>534</v>
+      </c>
+      <c r="C255" s="38"/>
+      <c r="D255" s="38">
         <v>8.0</v>
       </c>
-      <c r="E254" s="38"/>
-    </row>
-    <row r="255" ht="22.5" customHeight="1">
-      <c r="A255" s="39" t="s">
+      <c r="E255" s="38"/>
+    </row>
+    <row r="256" ht="22.5" customHeight="1">
+      <c r="A256" s="39" t="s">
         <v>536</v>
       </c>
-      <c r="B255" s="40"/>
-      <c r="C255" s="41"/>
-      <c r="D255" s="41">
+      <c r="B256" s="40"/>
+      <c r="C256" s="41"/>
+      <c r="D256" s="41">
         <v>4.0</v>
       </c>
-      <c r="E255" s="41"/>
-    </row>
-    <row r="256" ht="22.5" customHeight="1">
-      <c r="A256" s="37" t="s">
-        <v>915</v>
-      </c>
-      <c r="B256" s="45" t="s">
-        <v>536</v>
-      </c>
-      <c r="C256" s="38"/>
-      <c r="D256" s="38">
-        <v>12.0</v>
-      </c>
-      <c r="E256" s="38"/>
+      <c r="E256" s="41"/>
     </row>
     <row r="257" ht="22.5" customHeight="1">
       <c r="A257" s="37" t="s">
@@ -12605,7 +12606,7 @@
       </c>
       <c r="C257" s="38"/>
       <c r="D257" s="38">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="E257" s="38"/>
     </row>
@@ -12618,7 +12619,7 @@
       </c>
       <c r="C258" s="38"/>
       <c r="D258" s="38">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="E258" s="38"/>
     </row>
@@ -12631,7 +12632,7 @@
       </c>
       <c r="C259" s="38"/>
       <c r="D259" s="38">
-        <v>24.0</v>
+        <v>20.0</v>
       </c>
       <c r="E259" s="38"/>
     </row>
@@ -12644,7 +12645,7 @@
       </c>
       <c r="C260" s="38"/>
       <c r="D260" s="38">
-        <v>28.0</v>
+        <v>24.0</v>
       </c>
       <c r="E260" s="38"/>
     </row>
@@ -12657,7 +12658,7 @@
       </c>
       <c r="C261" s="38"/>
       <c r="D261" s="38">
-        <v>32.0</v>
+        <v>28.0</v>
       </c>
       <c r="E261" s="38"/>
     </row>
@@ -12670,7 +12671,7 @@
       </c>
       <c r="C262" s="38"/>
       <c r="D262" s="38">
-        <v>36.0</v>
+        <v>32.0</v>
       </c>
       <c r="E262" s="38"/>
     </row>
@@ -12683,7 +12684,7 @@
       </c>
       <c r="C263" s="38"/>
       <c r="D263" s="38">
-        <v>4.0</v>
+        <v>36.0</v>
       </c>
       <c r="E263" s="38"/>
     </row>
@@ -12696,7 +12697,7 @@
       </c>
       <c r="C264" s="38"/>
       <c r="D264" s="38">
-        <v>40.0</v>
+        <v>4.0</v>
       </c>
       <c r="E264" s="38"/>
     </row>
@@ -12709,7 +12710,7 @@
       </c>
       <c r="C265" s="38"/>
       <c r="D265" s="38">
-        <v>44.0</v>
+        <v>40.0</v>
       </c>
       <c r="E265" s="38"/>
     </row>
@@ -12722,7 +12723,7 @@
       </c>
       <c r="C266" s="38"/>
       <c r="D266" s="38">
-        <v>48.0</v>
+        <v>44.0</v>
       </c>
       <c r="E266" s="38"/>
     </row>
@@ -12735,33 +12736,33 @@
       </c>
       <c r="C267" s="38"/>
       <c r="D267" s="38">
+        <v>48.0</v>
+      </c>
+      <c r="E267" s="38"/>
+    </row>
+    <row r="268" ht="22.5" customHeight="1">
+      <c r="A268" s="37" t="s">
+        <v>927</v>
+      </c>
+      <c r="B268" s="45" t="s">
+        <v>536</v>
+      </c>
+      <c r="C268" s="38"/>
+      <c r="D268" s="38">
         <v>8.0</v>
       </c>
-      <c r="E267" s="38"/>
-    </row>
-    <row r="268" ht="22.5" customHeight="1">
-      <c r="A268" s="39" t="s">
+      <c r="E268" s="38"/>
+    </row>
+    <row r="269" ht="22.5" customHeight="1">
+      <c r="A269" s="39" t="s">
         <v>538</v>
       </c>
-      <c r="B268" s="40"/>
-      <c r="C268" s="41"/>
-      <c r="D268" s="41">
+      <c r="B269" s="40"/>
+      <c r="C269" s="41"/>
+      <c r="D269" s="41">
         <v>4.0</v>
       </c>
-      <c r="E268" s="41"/>
-    </row>
-    <row r="269" ht="22.5" customHeight="1">
-      <c r="A269" s="37" t="s">
-        <v>927</v>
-      </c>
-      <c r="B269" s="45" t="s">
-        <v>538</v>
-      </c>
-      <c r="C269" s="38"/>
-      <c r="D269" s="38">
-        <v>12.0</v>
-      </c>
-      <c r="E269" s="38"/>
+      <c r="E269" s="41"/>
     </row>
     <row r="270" ht="22.5" customHeight="1">
       <c r="A270" s="37" t="s">
@@ -12772,7 +12773,7 @@
       </c>
       <c r="C270" s="38"/>
       <c r="D270" s="38">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="E270" s="38"/>
     </row>
@@ -12785,7 +12786,7 @@
       </c>
       <c r="C271" s="38"/>
       <c r="D271" s="38">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="E271" s="38"/>
     </row>
@@ -12798,7 +12799,7 @@
       </c>
       <c r="C272" s="38"/>
       <c r="D272" s="38">
-        <v>24.0</v>
+        <v>20.0</v>
       </c>
       <c r="E272" s="38"/>
     </row>
@@ -12811,7 +12812,7 @@
       </c>
       <c r="C273" s="38"/>
       <c r="D273" s="38">
-        <v>28.0</v>
+        <v>24.0</v>
       </c>
       <c r="E273" s="38"/>
     </row>
@@ -12824,7 +12825,7 @@
       </c>
       <c r="C274" s="38"/>
       <c r="D274" s="38">
-        <v>36.0</v>
+        <v>28.0</v>
       </c>
       <c r="E274" s="38"/>
     </row>
@@ -12837,7 +12838,7 @@
       </c>
       <c r="C275" s="38"/>
       <c r="D275" s="38">
-        <v>4.0</v>
+        <v>36.0</v>
       </c>
       <c r="E275" s="38"/>
     </row>
@@ -12850,7 +12851,7 @@
       </c>
       <c r="C276" s="38"/>
       <c r="D276" s="38">
-        <v>40.0</v>
+        <v>4.0</v>
       </c>
       <c r="E276" s="38"/>
     </row>
@@ -12863,7 +12864,7 @@
       </c>
       <c r="C277" s="38"/>
       <c r="D277" s="38">
-        <v>32.0</v>
+        <v>40.0</v>
       </c>
       <c r="E277" s="38"/>
     </row>
@@ -12876,7 +12877,7 @@
       </c>
       <c r="C278" s="38"/>
       <c r="D278" s="38">
-        <v>44.0</v>
+        <v>32.0</v>
       </c>
       <c r="E278" s="38"/>
     </row>
@@ -12889,7 +12890,7 @@
       </c>
       <c r="C279" s="38"/>
       <c r="D279" s="38">
-        <v>48.0</v>
+        <v>44.0</v>
       </c>
       <c r="E279" s="38"/>
     </row>
@@ -12902,33 +12903,33 @@
       </c>
       <c r="C280" s="38"/>
       <c r="D280" s="38">
+        <v>48.0</v>
+      </c>
+      <c r="E280" s="38"/>
+    </row>
+    <row r="281" ht="22.5" customHeight="1">
+      <c r="A281" s="37" t="s">
+        <v>939</v>
+      </c>
+      <c r="B281" s="45" t="s">
+        <v>538</v>
+      </c>
+      <c r="C281" s="38"/>
+      <c r="D281" s="38">
         <v>8.0</v>
       </c>
-      <c r="E280" s="38"/>
-    </row>
-    <row r="281" ht="22.5" customHeight="1">
-      <c r="A281" s="39" t="s">
+      <c r="E281" s="38"/>
+    </row>
+    <row r="282" ht="22.5" customHeight="1">
+      <c r="A282" s="39" t="s">
         <v>540</v>
       </c>
-      <c r="B281" s="40"/>
-      <c r="C281" s="41"/>
-      <c r="D281" s="41">
+      <c r="B282" s="40"/>
+      <c r="C282" s="41"/>
+      <c r="D282" s="41">
         <v>4.0</v>
       </c>
-      <c r="E281" s="41"/>
-    </row>
-    <row r="282" ht="22.5" customHeight="1">
-      <c r="A282" s="37" t="s">
-        <v>939</v>
-      </c>
-      <c r="B282" s="45" t="s">
-        <v>540</v>
-      </c>
-      <c r="C282" s="38"/>
-      <c r="D282" s="38">
-        <v>12.0</v>
-      </c>
-      <c r="E282" s="38"/>
+      <c r="E282" s="41"/>
     </row>
     <row r="283" ht="22.5" customHeight="1">
       <c r="A283" s="37" t="s">
@@ -12939,7 +12940,7 @@
       </c>
       <c r="C283" s="38"/>
       <c r="D283" s="38">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="E283" s="38"/>
     </row>
@@ -12952,7 +12953,7 @@
       </c>
       <c r="C284" s="38"/>
       <c r="D284" s="38">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="E284" s="38"/>
     </row>
@@ -12965,7 +12966,7 @@
       </c>
       <c r="C285" s="38"/>
       <c r="D285" s="38">
-        <v>24.0</v>
+        <v>20.0</v>
       </c>
       <c r="E285" s="38"/>
     </row>
@@ -12978,7 +12979,7 @@
       </c>
       <c r="C286" s="38"/>
       <c r="D286" s="38">
-        <v>28.0</v>
+        <v>24.0</v>
       </c>
       <c r="E286" s="38"/>
     </row>
@@ -12991,7 +12992,7 @@
       </c>
       <c r="C287" s="38"/>
       <c r="D287" s="38">
-        <v>32.0</v>
+        <v>28.0</v>
       </c>
       <c r="E287" s="38"/>
     </row>
@@ -13004,7 +13005,7 @@
       </c>
       <c r="C288" s="38"/>
       <c r="D288" s="38">
-        <v>36.0</v>
+        <v>32.0</v>
       </c>
       <c r="E288" s="38"/>
     </row>
@@ -13017,7 +13018,7 @@
       </c>
       <c r="C289" s="38"/>
       <c r="D289" s="38">
-        <v>4.0</v>
+        <v>36.0</v>
       </c>
       <c r="E289" s="38"/>
     </row>
@@ -13030,7 +13031,7 @@
       </c>
       <c r="C290" s="38"/>
       <c r="D290" s="38">
-        <v>40.0</v>
+        <v>4.0</v>
       </c>
       <c r="E290" s="38"/>
     </row>
@@ -13043,7 +13044,7 @@
       </c>
       <c r="C291" s="38"/>
       <c r="D291" s="38">
-        <v>44.0</v>
+        <v>40.0</v>
       </c>
       <c r="E291" s="38"/>
     </row>
@@ -13056,7 +13057,7 @@
       </c>
       <c r="C292" s="38"/>
       <c r="D292" s="38">
-        <v>48.0</v>
+        <v>44.0</v>
       </c>
       <c r="E292" s="38"/>
     </row>
@@ -13069,33 +13070,33 @@
       </c>
       <c r="C293" s="38"/>
       <c r="D293" s="38">
+        <v>48.0</v>
+      </c>
+      <c r="E293" s="38"/>
+    </row>
+    <row r="294" ht="22.5" customHeight="1">
+      <c r="A294" s="37" t="s">
+        <v>951</v>
+      </c>
+      <c r="B294" s="45" t="s">
+        <v>540</v>
+      </c>
+      <c r="C294" s="38"/>
+      <c r="D294" s="38">
         <v>8.0</v>
       </c>
-      <c r="E293" s="38"/>
-    </row>
-    <row r="294" ht="22.5" customHeight="1">
-      <c r="A294" s="39" t="s">
+      <c r="E294" s="38"/>
+    </row>
+    <row r="295" ht="22.5" customHeight="1">
+      <c r="A295" s="39" t="s">
         <v>542</v>
       </c>
-      <c r="B294" s="40"/>
-      <c r="C294" s="41"/>
-      <c r="D294" s="41">
+      <c r="B295" s="40"/>
+      <c r="C295" s="41"/>
+      <c r="D295" s="41">
         <v>4.0</v>
       </c>
-      <c r="E294" s="41"/>
-    </row>
-    <row r="295" ht="22.5" customHeight="1">
-      <c r="A295" s="37" t="s">
-        <v>951</v>
-      </c>
-      <c r="B295" s="45" t="s">
-        <v>542</v>
-      </c>
-      <c r="C295" s="38"/>
-      <c r="D295" s="38">
-        <v>12.0</v>
-      </c>
-      <c r="E295" s="38"/>
+      <c r="E295" s="41"/>
     </row>
     <row r="296" ht="22.5" customHeight="1">
       <c r="A296" s="37" t="s">
@@ -13106,7 +13107,7 @@
       </c>
       <c r="C296" s="38"/>
       <c r="D296" s="38">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="E296" s="38"/>
     </row>
@@ -13119,7 +13120,7 @@
       </c>
       <c r="C297" s="38"/>
       <c r="D297" s="38">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="E297" s="38"/>
     </row>
@@ -13132,7 +13133,7 @@
       </c>
       <c r="C298" s="38"/>
       <c r="D298" s="38">
-        <v>24.0</v>
+        <v>20.0</v>
       </c>
       <c r="E298" s="38"/>
     </row>
@@ -13145,7 +13146,7 @@
       </c>
       <c r="C299" s="38"/>
       <c r="D299" s="38">
-        <v>28.0</v>
+        <v>24.0</v>
       </c>
       <c r="E299" s="38"/>
     </row>
@@ -13158,7 +13159,7 @@
       </c>
       <c r="C300" s="38"/>
       <c r="D300" s="38">
-        <v>32.0</v>
+        <v>28.0</v>
       </c>
       <c r="E300" s="38"/>
     </row>
@@ -13171,7 +13172,7 @@
       </c>
       <c r="C301" s="38"/>
       <c r="D301" s="38">
-        <v>36.0</v>
+        <v>32.0</v>
       </c>
       <c r="E301" s="38"/>
     </row>
@@ -13184,7 +13185,7 @@
       </c>
       <c r="C302" s="38"/>
       <c r="D302" s="38">
-        <v>4.0</v>
+        <v>36.0</v>
       </c>
       <c r="E302" s="38"/>
     </row>
@@ -13197,7 +13198,7 @@
       </c>
       <c r="C303" s="38"/>
       <c r="D303" s="38">
-        <v>40.0</v>
+        <v>4.0</v>
       </c>
       <c r="E303" s="38"/>
     </row>
@@ -13210,7 +13211,7 @@
       </c>
       <c r="C304" s="38"/>
       <c r="D304" s="38">
-        <v>44.0</v>
+        <v>40.0</v>
       </c>
       <c r="E304" s="38"/>
     </row>
@@ -13223,7 +13224,7 @@
       </c>
       <c r="C305" s="38"/>
       <c r="D305" s="38">
-        <v>48.0</v>
+        <v>44.0</v>
       </c>
       <c r="E305" s="38"/>
     </row>
@@ -13236,33 +13237,33 @@
       </c>
       <c r="C306" s="38"/>
       <c r="D306" s="38">
+        <v>48.0</v>
+      </c>
+      <c r="E306" s="38"/>
+    </row>
+    <row r="307" ht="22.5" customHeight="1">
+      <c r="A307" s="37" t="s">
+        <v>963</v>
+      </c>
+      <c r="B307" s="45" t="s">
+        <v>542</v>
+      </c>
+      <c r="C307" s="38"/>
+      <c r="D307" s="38">
         <v>8.0</v>
       </c>
-      <c r="E306" s="38"/>
-    </row>
-    <row r="307" ht="22.5" customHeight="1">
-      <c r="A307" s="39" t="s">
+      <c r="E307" s="38"/>
+    </row>
+    <row r="308" ht="22.5" customHeight="1">
+      <c r="A308" s="39" t="s">
         <v>544</v>
       </c>
-      <c r="B307" s="40"/>
-      <c r="C307" s="41"/>
-      <c r="D307" s="41">
+      <c r="B308" s="40"/>
+      <c r="C308" s="41"/>
+      <c r="D308" s="41">
         <v>4.0</v>
       </c>
-      <c r="E307" s="41"/>
-    </row>
-    <row r="308" ht="22.5" customHeight="1">
-      <c r="A308" s="37" t="s">
-        <v>963</v>
-      </c>
-      <c r="B308" s="45" t="s">
-        <v>544</v>
-      </c>
-      <c r="C308" s="38"/>
-      <c r="D308" s="38">
-        <v>12.0</v>
-      </c>
-      <c r="E308" s="38"/>
+      <c r="E308" s="41"/>
     </row>
     <row r="309" ht="22.5" customHeight="1">
       <c r="A309" s="37" t="s">
@@ -13273,7 +13274,7 @@
       </c>
       <c r="C309" s="38"/>
       <c r="D309" s="38">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="E309" s="38"/>
     </row>
@@ -13286,7 +13287,7 @@
       </c>
       <c r="C310" s="38"/>
       <c r="D310" s="38">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="E310" s="38"/>
     </row>
@@ -13299,7 +13300,7 @@
       </c>
       <c r="C311" s="38"/>
       <c r="D311" s="38">
-        <v>24.0</v>
+        <v>20.0</v>
       </c>
       <c r="E311" s="38"/>
     </row>
@@ -13312,7 +13313,7 @@
       </c>
       <c r="C312" s="38"/>
       <c r="D312" s="38">
-        <v>28.0</v>
+        <v>24.0</v>
       </c>
       <c r="E312" s="38"/>
     </row>
@@ -13325,7 +13326,7 @@
       </c>
       <c r="C313" s="38"/>
       <c r="D313" s="38">
-        <v>32.0</v>
+        <v>28.0</v>
       </c>
       <c r="E313" s="38"/>
     </row>
@@ -13338,7 +13339,7 @@
       </c>
       <c r="C314" s="38"/>
       <c r="D314" s="38">
-        <v>36.0</v>
+        <v>32.0</v>
       </c>
       <c r="E314" s="38"/>
     </row>
@@ -13351,7 +13352,7 @@
       </c>
       <c r="C315" s="38"/>
       <c r="D315" s="38">
-        <v>4.0</v>
+        <v>36.0</v>
       </c>
       <c r="E315" s="38"/>
     </row>
@@ -13364,7 +13365,7 @@
       </c>
       <c r="C316" s="38"/>
       <c r="D316" s="38">
-        <v>40.0</v>
+        <v>4.0</v>
       </c>
       <c r="E316" s="38"/>
     </row>
@@ -13377,7 +13378,7 @@
       </c>
       <c r="C317" s="38"/>
       <c r="D317" s="38">
-        <v>44.0</v>
+        <v>40.0</v>
       </c>
       <c r="E317" s="38"/>
     </row>
@@ -13390,7 +13391,7 @@
       </c>
       <c r="C318" s="38"/>
       <c r="D318" s="38">
-        <v>48.0</v>
+        <v>44.0</v>
       </c>
       <c r="E318" s="38"/>
     </row>
@@ -13403,27 +13404,29 @@
       </c>
       <c r="C319" s="38"/>
       <c r="D319" s="38">
+        <v>48.0</v>
+      </c>
+      <c r="E319" s="38"/>
+    </row>
+    <row r="320" ht="22.5" customHeight="1">
+      <c r="A320" s="37" t="s">
+        <v>975</v>
+      </c>
+      <c r="B320" s="45" t="s">
+        <v>544</v>
+      </c>
+      <c r="C320" s="38"/>
+      <c r="D320" s="38">
         <v>8.0</v>
       </c>
-      <c r="E319" s="38"/>
-    </row>
-    <row r="320" ht="22.5" customHeight="1">
-      <c r="A320" s="28" t="s">
-        <v>975</v>
-      </c>
-      <c r="B320" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="C320" s="29"/>
-      <c r="D320" s="29"/>
-      <c r="E320" s="29"/>
+      <c r="E320" s="38"/>
     </row>
     <row r="321" ht="22.5" customHeight="1">
       <c r="A321" s="28" t="s">
         <v>976</v>
       </c>
       <c r="B321" s="28" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C321" s="29"/>
       <c r="D321" s="29"/>
@@ -13434,18 +13437,22 @@
         <v>977</v>
       </c>
       <c r="B322" s="28" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C322" s="29"/>
       <c r="D322" s="29"/>
       <c r="E322" s="29"/>
     </row>
-    <row r="323">
-      <c r="A323" s="47"/>
-      <c r="B323" s="48"/>
-      <c r="C323" s="49"/>
-      <c r="D323" s="49"/>
-      <c r="E323" s="49"/>
+    <row r="323" ht="22.5" customHeight="1">
+      <c r="A323" s="28" t="s">
+        <v>978</v>
+      </c>
+      <c r="B323" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C323" s="29"/>
+      <c r="D323" s="29"/>
+      <c r="E323" s="29"/>
     </row>
     <row r="324">
       <c r="A324" s="47"/>
@@ -17611,6 +17618,13 @@
       <c r="C918" s="49"/>
       <c r="D918" s="49"/>
       <c r="E918" s="49"/>
+    </row>
+    <row r="919">
+      <c r="A919" s="47"/>
+      <c r="B919" s="48"/>
+      <c r="C919" s="49"/>
+      <c r="D919" s="49"/>
+      <c r="E919" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -17663,24 +17677,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="50" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="51" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="D2" s="52"/>
       <c r="E2" s="52"/>
@@ -17708,13 +17722,13 @@
     </row>
     <row r="3">
       <c r="A3" s="51" t="s">
+        <v>984</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>759</v>
+      </c>
+      <c r="C3" s="51" t="s">
         <v>983</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>758</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>982</v>
       </c>
       <c r="D3" s="52"/>
       <c r="E3" s="52"/>
@@ -17742,275 +17756,275 @@
     </row>
     <row r="4">
       <c r="A4" s="53" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="53" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B5" s="53" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="53" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="53" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B7" s="53" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="53" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="53" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B9" s="53" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="53" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="53" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="53" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B12" s="53" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="53" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="53" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C14" s="53" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="53" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C15" s="53" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="53" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="53" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B17" s="53" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C17" s="53" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="53" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B18" s="53" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C18" s="53" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="53" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C19" s="53" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="53" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C20" s="53" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="53" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B21" s="53" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="53" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B22" s="53" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C22" s="53" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="53" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B23" s="53" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C23" s="53" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="53" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B24" s="53" t="s">
         <v>707</v>
       </c>
       <c r="C24" s="53" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="53" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C25" s="53" t="s">
         <v>1012</v>
-      </c>
-      <c r="B25" s="53" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C25" s="53" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="53" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B26" s="53" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C26" s="53" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="53" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B27" s="53" t="s">
         <v>708</v>
       </c>
       <c r="C27" s="53" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="54" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B28" s="55"/>
       <c r="C28" s="54" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="D28" s="56"/>
       <c r="E28" s="56"/>
@@ -18038,11 +18052,11 @@
     </row>
     <row r="29">
       <c r="A29" s="57" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B29" s="58"/>
       <c r="C29" s="57" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
@@ -18070,11 +18084,11 @@
     </row>
     <row r="30">
       <c r="A30" s="57" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B30" s="58"/>
       <c r="C30" s="57" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="D30" s="59"/>
       <c r="E30" s="59"/>
@@ -18102,11 +18116,11 @@
     </row>
     <row r="31">
       <c r="A31" s="57" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B31" s="58"/>
       <c r="C31" s="57" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
@@ -18134,11 +18148,11 @@
     </row>
     <row r="32">
       <c r="A32" s="57" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B32" s="58"/>
       <c r="C32" s="57" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="D32" s="59"/>
       <c r="E32" s="59"/>
@@ -18166,11 +18180,11 @@
     </row>
     <row r="33">
       <c r="A33" s="54" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B33" s="55"/>
       <c r="C33" s="54" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="D33" s="56"/>
       <c r="E33" s="56"/>
@@ -18198,102 +18212,102 @@
     </row>
     <row r="34">
       <c r="A34" s="53" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B34" s="53" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C34" s="53" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="53" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B35" s="53" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="53" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B36" s="53" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C36" s="53" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="53" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B37" s="53" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C37" s="53" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="53" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B38" s="53" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="53" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B39" s="60"/>
       <c r="C39" s="53" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="53" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B40" s="60"/>
       <c r="C40" s="53" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="53" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B41" s="60"/>
       <c r="C41" s="53" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="53" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B42" s="60"/>
       <c r="C42" s="53" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="54" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B43" s="55"/>
       <c r="C43" s="54" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="D43" s="56"/>
       <c r="E43" s="56"/>
@@ -18321,11 +18335,11 @@
     </row>
     <row r="44">
       <c r="A44" s="54" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B44" s="55"/>
       <c r="C44" s="54" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="D44" s="56"/>
       <c r="E44" s="56"/>
@@ -18353,11 +18367,11 @@
     </row>
     <row r="45">
       <c r="A45" s="54" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B45" s="55"/>
       <c r="C45" s="54" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="D45" s="56"/>
       <c r="E45" s="56"/>
@@ -18385,11 +18399,11 @@
     </row>
     <row r="46">
       <c r="A46" s="54" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B46" s="55"/>
       <c r="C46" s="54" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="D46" s="56"/>
       <c r="E46" s="56"/>
@@ -18417,11 +18431,11 @@
     </row>
     <row r="47">
       <c r="A47" s="54" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B47" s="55"/>
       <c r="C47" s="54" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="D47" s="56"/>
       <c r="E47" s="56"/>
@@ -18449,11 +18463,11 @@
     </row>
     <row r="48">
       <c r="A48" s="54" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B48" s="55"/>
       <c r="C48" s="54" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="D48" s="56"/>
       <c r="E48" s="56"/>
@@ -18481,11 +18495,11 @@
     </row>
     <row r="49">
       <c r="A49" s="54" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B49" s="55"/>
       <c r="C49" s="54" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="D49" s="56"/>
       <c r="E49" s="56"/>
@@ -18540,12 +18554,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="62" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="D1" s="63"/>
       <c r="E1" s="64"/>
       <c r="F1" s="62" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="G1" s="63"/>
       <c r="H1" s="64"/>
@@ -18554,22 +18568,22 @@
       <c r="A2" s="65"/>
       <c r="B2" s="65"/>
       <c r="C2" s="66" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="D2" s="66" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F2" s="66" t="s">
         <v>1036</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="G2" s="66" t="s">
         <v>1037</v>
       </c>
-      <c r="F2" s="66" t="s">
-        <v>1035</v>
-      </c>
-      <c r="G2" s="66" t="s">
-        <v>1036</v>
-      </c>
       <c r="H2" s="66" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="3">
@@ -18755,7 +18769,7 @@
     </row>
     <row r="12">
       <c r="A12" s="67" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B12" s="67" t="s">
         <v>37</v>
@@ -18776,7 +18790,7 @@
     </row>
     <row r="13">
       <c r="A13" s="67" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B13" s="67" t="s">
         <v>39</v>
@@ -18797,7 +18811,7 @@
     </row>
     <row r="14">
       <c r="A14" s="67" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B14" s="67" t="s">
         <v>41</v>
@@ -18894,7 +18908,7 @@
     </row>
     <row r="19">
       <c r="A19" s="67" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B19" s="67" t="s">
         <v>47</v>
@@ -18911,7 +18925,7 @@
     </row>
     <row r="20">
       <c r="A20" s="67" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B20" s="67" t="s">
         <v>153</v>
@@ -18962,7 +18976,7 @@
     </row>
     <row r="23">
       <c r="A23" s="67" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B23" s="67" t="s">
         <v>67</v>
@@ -18979,7 +18993,7 @@
     </row>
     <row r="24">
       <c r="A24" s="67" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B24" s="67" t="s">
         <v>69</v>
@@ -18996,7 +19010,7 @@
     </row>
     <row r="25">
       <c r="A25" s="67" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B25" s="67" t="s">
         <v>71</v>
@@ -19013,7 +19027,7 @@
     </row>
     <row r="26">
       <c r="A26" s="67" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B26" s="67" t="s">
         <v>73</v>
@@ -19030,7 +19044,7 @@
     </row>
     <row r="27">
       <c r="A27" s="67" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B27" s="67" t="s">
         <v>75</v>
@@ -19047,7 +19061,7 @@
     </row>
     <row r="28">
       <c r="A28" s="67" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B28" s="67" t="s">
         <v>77</v>
@@ -19515,7 +19529,7 @@
     </row>
     <row r="52">
       <c r="A52" s="67" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B52" s="67" t="s">
         <v>149</v>
@@ -19532,7 +19546,7 @@
     </row>
     <row r="53">
       <c r="A53" s="67" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B53" s="67" t="s">
         <v>151</v>
@@ -19706,10 +19720,10 @@
     </row>
     <row r="63">
       <c r="A63" s="67" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B63" s="67" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="C63" s="69"/>
       <c r="D63" s="69"/>
@@ -21438,7 +21452,7 @@
     </row>
     <row r="163">
       <c r="A163" s="67" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B163" s="67" t="s">
         <v>535</v>
@@ -21458,7 +21472,7 @@
         <v>604</v>
       </c>
       <c r="B164" s="67" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C164" s="69"/>
       <c r="D164" s="69"/>

</xml_diff>